<commit_message>
executed experiment on chw-work
</commit_message>
<xml_diff>
--- a/test/panalysis/kieker/evaluation.xlsx
+++ b/test/panalysis/kieker/evaluation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>test name</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>chw-work</t>
+  </si>
+  <si>
+    <t>optimierungen</t>
+  </si>
+  <si>
+    <t>put+take</t>
   </si>
 </sst>
 </file>
@@ -130,9 +136,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K13" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K13"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:L13"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="PC"/>
     <tableColumn id="2" name="test name"/>
     <tableColumn id="3" name="NUM_OBJECTS_TO_CREATE" dataDxfId="0"/>
@@ -144,6 +150,7 @@
     <tableColumn id="9" name="75% (µs)"/>
     <tableColumn id="10" name="100% (µs)"/>
     <tableColumn id="11" name="confidenceWidth (in µs)"/>
+    <tableColumn id="12" name="optimierungen"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +462,7 @@
     <col min="11" max="11" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -489,8 +496,11 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -525,7 +535,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -560,7 +570,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -594,16 +604,49 @@
       <c r="K4">
         <v>1.486</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
       <c r="C5" s="1">
         <v>100000</v>
       </c>
       <c r="D5">
         <v>800</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>634</v>
+      </c>
+      <c r="F5">
+        <v>453</v>
+      </c>
+      <c r="G5">
+        <v>475</v>
+      </c>
+      <c r="H5">
+        <v>493</v>
+      </c>
+      <c r="I5">
+        <v>564</v>
+      </c>
+      <c r="J5">
+        <v>3237</v>
+      </c>
+      <c r="K5">
+        <v>2.9140000000000001</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -638,7 +681,7 @@
         <v>0.42099999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -673,7 +716,7 @@
         <v>0.45400000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -708,7 +751,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -743,7 +786,7 @@
         <v>0.78400000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -778,7 +821,7 @@
         <v>0.60699999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -813,7 +856,7 @@
         <v>1.1830000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -848,7 +891,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>

</xml_diff>